<commit_message>
Added autotests, Result.md, new README.md, allure-results.zip
</commit_message>
<xml_diff>
--- a/Cases.xlsx
+++ b/Cases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Netology\DIPLOMQA\fmh_android_15_03_24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9B9F7F-1B81-4743-916B-5BECE40FAB09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1BF625A-8B27-443A-B5FD-C24C6BEDDB8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="879" uniqueCount="372">
   <si>
     <t>Комментарий</t>
   </si>
@@ -1801,9 +1801,9 @@
   <dimension ref="A1:K347"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A185" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A248" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="C141" sqref="C141:C143"/>
+      <selection pane="bottomLeft" activeCell="J258" sqref="J258:J261"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1968,7 +1968,9 @@
         <v>18</v>
       </c>
       <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
+      <c r="J7" s="18" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="8" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A8" s="12"/>
@@ -1984,7 +1986,7 @@
       </c>
       <c r="H8" s="19"/>
       <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
+      <c r="J8" s="19"/>
     </row>
     <row r="9" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
@@ -2000,7 +2002,7 @@
       </c>
       <c r="H9" s="19"/>
       <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
+      <c r="J9" s="19"/>
     </row>
     <row r="10" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A10" s="12"/>
@@ -2016,7 +2018,7 @@
       </c>
       <c r="H10" s="29"/>
       <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
+      <c r="J10" s="29"/>
     </row>
     <row r="11" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A11" s="12">
@@ -2042,7 +2044,9 @@
         <v>18</v>
       </c>
       <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
+      <c r="J11" s="18" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="12" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A12" s="12"/>
@@ -2058,7 +2062,7 @@
       </c>
       <c r="H12" s="19"/>
       <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
+      <c r="J12" s="19"/>
     </row>
     <row r="13" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
@@ -2074,7 +2078,7 @@
       </c>
       <c r="H13" s="19"/>
       <c r="I13" s="14"/>
-      <c r="J13" s="14"/>
+      <c r="J13" s="19"/>
     </row>
     <row r="14" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A14" s="12"/>
@@ -2090,7 +2094,7 @@
       </c>
       <c r="H14" s="29"/>
       <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
+      <c r="J14" s="29"/>
     </row>
     <row r="15" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A15" s="12">
@@ -2116,7 +2120,9 @@
         <v>18</v>
       </c>
       <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
+      <c r="J15" s="18" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="12"/>
@@ -2132,7 +2138,7 @@
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
+      <c r="J16" s="19"/>
     </row>
     <row r="17" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
@@ -2148,7 +2154,7 @@
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
+      <c r="J17" s="19"/>
     </row>
     <row r="18" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
@@ -2164,7 +2170,7 @@
       </c>
       <c r="H18" s="29"/>
       <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
+      <c r="J18" s="29"/>
     </row>
     <row r="19" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A19" s="12">
@@ -2268,7 +2274,9 @@
         <v>18</v>
       </c>
       <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
+      <c r="J23" s="18" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="24" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A24" s="12"/>
@@ -2284,7 +2292,7 @@
       </c>
       <c r="H24" s="19"/>
       <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
+      <c r="J24" s="19"/>
     </row>
     <row r="25" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
@@ -2300,7 +2308,7 @@
       </c>
       <c r="H25" s="19"/>
       <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
+      <c r="J25" s="19"/>
     </row>
     <row r="26" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A26" s="12"/>
@@ -2316,7 +2324,7 @@
       </c>
       <c r="H26" s="29"/>
       <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
+      <c r="J26" s="29"/>
     </row>
     <row r="27" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A27" s="12">
@@ -2342,7 +2350,9 @@
         <v>18</v>
       </c>
       <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
+      <c r="J27" s="18" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="28" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A28" s="12"/>
@@ -2358,7 +2368,7 @@
       </c>
       <c r="H28" s="19"/>
       <c r="I28" s="14"/>
-      <c r="J28" s="14"/>
+      <c r="J28" s="19"/>
     </row>
     <row r="29" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A29" s="12"/>
@@ -2374,7 +2384,7 @@
       </c>
       <c r="H29" s="19"/>
       <c r="I29" s="14"/>
-      <c r="J29" s="14"/>
+      <c r="J29" s="19"/>
     </row>
     <row r="30" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A30" s="12"/>
@@ -2390,7 +2400,7 @@
       </c>
       <c r="H30" s="29"/>
       <c r="I30" s="14"/>
-      <c r="J30" s="14"/>
+      <c r="J30" s="29"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="27" t="s">
@@ -2430,7 +2440,9 @@
         <v>18</v>
       </c>
       <c r="I32" s="14"/>
-      <c r="J32" s="14"/>
+      <c r="J32" s="14" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="33" spans="1:10" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="12"/>
@@ -2472,7 +2484,9 @@
         <v>18</v>
       </c>
       <c r="I34" s="14"/>
-      <c r="J34" s="14"/>
+      <c r="J34" s="14" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="35" spans="1:10" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12"/>
@@ -2514,7 +2528,9 @@
         <v>18</v>
       </c>
       <c r="I36" s="14"/>
-      <c r="J36" s="14"/>
+      <c r="J36" s="14" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="37" spans="1:10" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="12"/>
@@ -2556,7 +2572,9 @@
         <v>18</v>
       </c>
       <c r="I38" s="14"/>
-      <c r="J38" s="14"/>
+      <c r="J38" s="14" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="39" spans="1:10" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="12"/>
@@ -2728,7 +2746,9 @@
         <v>18</v>
       </c>
       <c r="I47" s="18"/>
-      <c r="J47" s="37"/>
+      <c r="J47" s="14" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="48" spans="1:10" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="36"/>
@@ -2744,7 +2764,7 @@
       </c>
       <c r="H48" s="40"/>
       <c r="I48" s="29"/>
-      <c r="J48" s="38"/>
+      <c r="J48" s="14"/>
     </row>
     <row r="49" spans="1:10" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="12">
@@ -2844,7 +2864,9 @@
         <v>18</v>
       </c>
       <c r="I53" s="14"/>
-      <c r="J53" s="14"/>
+      <c r="J53" s="14" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="54" spans="1:10" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A54" s="12"/>
@@ -2902,7 +2924,9 @@
         <v>18</v>
       </c>
       <c r="I56" s="14"/>
-      <c r="J56" s="14"/>
+      <c r="J56" s="14" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="57" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="12"/>
@@ -2944,7 +2968,9 @@
         <v>18</v>
       </c>
       <c r="I58" s="14"/>
-      <c r="J58" s="14"/>
+      <c r="J58" s="14" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="59" spans="1:10" ht="51.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="12"/>
@@ -3132,7 +3158,9 @@
         <v>18</v>
       </c>
       <c r="I68" s="14"/>
-      <c r="J68" s="14"/>
+      <c r="J68" s="14" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="69" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="12"/>
@@ -3402,7 +3430,9 @@
         <v>18</v>
       </c>
       <c r="I83" s="14"/>
-      <c r="J83" s="14"/>
+      <c r="J83" s="14" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="84" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="12"/>
@@ -3556,7 +3586,9 @@
         <v>18</v>
       </c>
       <c r="I92" s="14"/>
-      <c r="J92" s="14"/>
+      <c r="J92" s="14" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="93" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="12"/>
@@ -3630,7 +3662,9 @@
         <v>18</v>
       </c>
       <c r="I96" s="14"/>
-      <c r="J96" s="14"/>
+      <c r="J96" s="14" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="97" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="12"/>
@@ -3736,7 +3770,9 @@
         <v>18</v>
       </c>
       <c r="I102" s="14"/>
-      <c r="J102" s="14"/>
+      <c r="J102" s="14" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="103" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="12"/>
@@ -4170,7 +4206,9 @@
         <v>18</v>
       </c>
       <c r="I127" s="14"/>
-      <c r="J127" s="14"/>
+      <c r="J127" s="14" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="128" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="12"/>
@@ -4338,7 +4376,9 @@
         <v>18</v>
       </c>
       <c r="I137" s="14"/>
-      <c r="J137" s="14"/>
+      <c r="J137" s="14" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="138" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="12"/>
@@ -4602,7 +4642,9 @@
         <v>18</v>
       </c>
       <c r="I151" s="14"/>
-      <c r="J151" s="14"/>
+      <c r="J151" s="14" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="152" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A152" s="12"/>
@@ -5664,7 +5706,9 @@
         <v>18</v>
       </c>
       <c r="I210" s="14"/>
-      <c r="J210" s="14"/>
+      <c r="J210" s="14" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="211" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A211" s="12"/>
@@ -5866,7 +5910,9 @@
         <v>18</v>
       </c>
       <c r="I222" s="14"/>
-      <c r="J222" s="14"/>
+      <c r="J222" s="14" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="223" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A223" s="12"/>
@@ -5958,7 +6004,9 @@
       <c r="I227" s="14" t="s">
         <v>286</v>
       </c>
-      <c r="J227" s="14"/>
+      <c r="J227" s="14" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="228" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A228" s="12"/>
@@ -6504,7 +6552,9 @@
       <c r="I258" s="14" t="s">
         <v>318</v>
       </c>
-      <c r="J258" s="14"/>
+      <c r="J258" s="14" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="259" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="12"/>
@@ -6580,7 +6630,9 @@
       <c r="I262" s="14" t="s">
         <v>318</v>
       </c>
-      <c r="J262" s="14"/>
+      <c r="J262" s="14" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="263" spans="1:10" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A263" s="12"/>
@@ -6654,7 +6706,9 @@
         <v>18</v>
       </c>
       <c r="I266" s="14"/>
-      <c r="J266" s="14"/>
+      <c r="J266" s="14" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="267" spans="1:10" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A267" s="12"/>

</xml_diff>